<commit_message>
Atualização automática de SANTIAGO.xlsx
</commit_message>
<xml_diff>
--- a/SANTIAGO.xlsx
+++ b/SANTIAGO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB2754B3-5DBD-4560-B6B5-E68087DA9924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC0C06B7-BC06-4F84-85B5-F8D15F8951D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1356,7 +1356,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{1731E67E-2925-42BD-953D-4C400CFA499F}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{9F622779-BBE5-44C7-B0AC-369E5C84D4BE}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1386,10 +1386,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0580646-A5DA-474F-9844-2BE8DB370532}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD4E1148-B1EB-4F71-948C-89EF5C1496CC}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1427,7 +1427,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A023AB6E-6950-4B9B-8D78-3058B5DA831C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65E98C07-F9CA-4191-8873-D5C1CE88335C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1490,7 +1490,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F4DDDD-5F21-4788-B7A5-860DCB82352A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D09064D2-4039-4028-AF74-5CE81C5C0AE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1509,7 +1509,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2F4FA55-4605-845D-4C5A-4C5F97EECE50}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{225830E6-52D3-AAF2-8AC3-BD51939279A2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1558,7 +1558,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{596A1154-BF6B-0D95-1C5E-A9512E93E5F5}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94A581AA-B786-407C-4DC6-6FB7754D7D5F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1577,7 +1577,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3D0059A-EB7C-4550-7689-059422162613}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A27FFCE3-9497-9A06-DBC9-866DEBF58661}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1608,7 +1608,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D620A9B-EEA6-51C7-6B59-C786AA6F9EAC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA5AB0C4-FA03-4C13-BE50-6E7DEEC9B714}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1639,7 +1639,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC539FEA-7ED6-874A-D24C-745C21F2BB94}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF784AA2-1F42-4B74-1D22-7832CC8E86F8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1682,7 +1682,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB9B1657-B2D8-4D40-92CA-1169F5FEC6DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21544655-798B-48EB-8E5C-F643A892BBB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1720,7 +1720,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCDFDAAD-809F-42D1-B6CF-6BF17630E1AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{276AC93F-B8C6-4D20-8D1E-3FF4D5A9F807}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1763,7 +1763,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EB1FB80-9BE4-47E1-99E6-DE13F4359C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9255451-74A3-45E5-BD48-B517EEE3C367}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2076,7 +2076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB88CB2-2A8A-4FEA-99B1-ADD80A4D7D30}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55179FF-7668-4032-98C8-4AE56FC990A1}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>